<commit_message>
update before re-submission with phylog. tree
</commit_message>
<xml_diff>
--- a/analysis/KEGG_raw_data/PNA79_16h_vs_H2O_16h_KEGG_FNN_16h.xlsx
+++ b/analysis/KEGG_raw_data/PNA79_16h_vs_H2O_16h_KEGG_FNN_16h.xlsx
@@ -47,12 +47,12 @@
     <t>fnu04980</t>
   </si>
   <si>
+    <t>fnu03070</t>
+  </si>
+  <si>
     <t>fnu03440</t>
   </si>
   <si>
-    <t>fnu03070</t>
-  </si>
-  <si>
     <t>fnu02060</t>
   </si>
   <si>
@@ -296,15 +296,15 @@
     <t>fnu00330</t>
   </si>
   <si>
+    <t>fnu01501</t>
+  </si>
+  <si>
     <t>fnu00270</t>
   </si>
   <si>
     <t>fnu00521</t>
   </si>
   <si>
-    <t>fnu01501</t>
-  </si>
-  <si>
     <t>fnu00052</t>
   </si>
   <si>
@@ -338,12 +338,12 @@
     <t>Cobalamin transport and metabolism</t>
   </si>
   <si>
+    <t>Bacterial secretion system</t>
+  </si>
+  <si>
     <t>Homologous recombination</t>
   </si>
   <si>
-    <t>Bacterial secretion system</t>
-  </si>
-  <si>
     <t>Phosphotransferase system (PTS)</t>
   </si>
   <si>
@@ -584,15 +584,15 @@
     <t>Arginine and proline metabolism</t>
   </si>
   <si>
+    <t>beta-Lactam resistance</t>
+  </si>
+  <si>
     <t>Cysteine and methionine metabolism</t>
   </si>
   <si>
     <t>Streptomycin biosynthesis</t>
   </si>
   <si>
-    <t>beta-Lactam resistance</t>
-  </si>
-  <si>
     <t>Galactose metabolism</t>
   </si>
   <si>
@@ -620,12 +620,12 @@
     <t>cds-C4N14_04180;cds-C4N14_05600</t>
   </si>
   <si>
+    <t>cds-C4N14_02370;cds-C4N14_09550;cds-C4N14_08725;cds-C4N14_08720;cds-C4N14_06785;cds-C4N14_05765;cds-C4N14_05425;cds-C4N14_10405;cds-C4N14_00680;cds-C4N14_01180;cds-C4N14_01890;cds-C4N14_02100;cds-C4N14_02135;cds-C4N14_02145</t>
+  </si>
+  <si>
     <t>cds-C4N14_04335;cds-C4N14_04465;cds-C4N14_04760;cds-C4N14_05260;cds-C4N14_10095;cds-C4N14_09560;cds-C4N14_09505;cds-C4N14_09150;cds-C4N14_07585;cds-C4N14_06635;cds-C4N14_06360;cds-C4N14_06045;cds-C4N14_05595;cds-C4N14_10345;cds-C4N14_10885;cds-C4N14_00445;cds-C4N14_00855;cds-C4N14_03915;cds-C4N14_02900;cds-C4N14_02340</t>
   </si>
   <si>
-    <t>cds-C4N14_02370;cds-C4N14_09550;cds-C4N14_08725;cds-C4N14_08720;cds-C4N14_06785;cds-C4N14_05425;cds-C4N14_10405;cds-C4N14_00680;cds-C4N14_01180;cds-C4N14_01890;cds-C4N14_02100;cds-C4N14_02135;cds-C4N14_02145</t>
-  </si>
-  <si>
     <t>cds-C4N14_09095;cds-C4N14_09090;cds-C4N14_09080;cds-C4N14_07595;cds-C4N14_10630;cds-C4N14_10635;cds-C4N14_10880;cds-C4N14_00270;cds-C4N14_01480;cds-C4N14_01530;cds-C4N14_01535;cds-C4N14_03445</t>
   </si>
   <si>
@@ -665,7 +665,7 @@
     <t>cds-C4N14_06380;cds-C4N14_06270;cds-C4N14_10535</t>
   </si>
   <si>
-    <t>cds-C4N14_02390;cds-C4N14_02395;cds-C4N14_02400;cds-C4N14_02450;cds-C4N14_02565;cds-C4N14_02625;cds-C4N14_02635;cds-C4N14_02695;cds-C4N14_02740;cds-C4N14_02745;cds-C4N14_02770;cds-C4N14_02775;cds-C4N14_02780;cds-C4N14_02800;cds-C4N14_02805;cds-C4N14_01785;cds-C4N14_01780;cds-C4N14_04115;cds-C4N14_04120;cds-C4N14_04125;cds-C4N14_04130;cds-C4N14_04135;cds-C4N14_04160;cds-C4N14_04180;cds-C4N14_04250;cds-C4N14_04385;cds-C4N14_04390;cds-C4N14_04395;cds-C4N14_04400;cds-C4N14_04460;cds-C4N14_04570;cds-C4N14_04575;cds-C4N14_04670;cds-C4N14_04695;cds-C4N14_04720;cds-C4N14_04725;cds-C4N14_04745;cds-C4N14_04795;cds-C4N14_04810;cds-C4N14_04815;cds-C4N14_04880;cds-C4N14_04920;cds-C4N14_04955;cds-C4N14_05010;cds-C4N14_05135;cds-C4N14_05140;cds-C4N14_05175;cds-C4N14_05180;cds-C4N14_05185;cds-C4N14_05190;cds-C4N14_05195;cds-C4N14_05200;cds-C4N14_05205;cds-C4N14_05210;cds-C4N14_05215;cds-C4N14_05220;cds-C4N14_05230;cds-C4N14_05240;cds-C4N14_05280;cds-C4N14_10125;cds-C4N14_10115;cds-C4N14_10110;cds-C4N14_10105;cds-C4N14_10085;cds-C4N14_10080;cds-C4N14_10075;cds-C4N14_10070;cds-C4N14_10065;cds-C4N14_10060;cds-C4N14_10055;cds-C4N14_10045;cds-C4N14_10040;cds-C4N14_10035;cds-C4N14_10005;cds-C4N14_09985;cds-C4N14_09965;cds-C4N14_09955;cds-C4N14_09925;cds-C4N14_09835;cds-C4N14_09810;cds-C4N14_09805;cds-C4N14_09785;cds-C4N14_09770;cds-C4N14_09755;cds-C4N14_09750;cds-C4N14_09725;cds-C4N14_09720;cds-C4N14_09685;cds-C4N14_09605;cds-C4N14_09555;cds-C4N14_09545;cds-C4N14_09540;cds-C4N14_09520;cds-C4N14_09465;cds-C4N14_09430;cds-C4N14_09330;cds-C4N14_09265;cds-C4N14_09260;cds-C4N14_09255;cds-C4N14_09250;cds-C4N14_09245;cds-C4N14_09135;cds-C4N14_09115;cds-C4N14_09020;cds-C4N14_09015;cds-C4N14_09010;cds-C4N14_08980;cds-C4N14_08970;cds-C4N14_08930;cds-C4N14_08920;cds-C4N14_08830;cds-C4N14_08825;cds-C4N14_08805;cds-C4N14_08690;cds-C4N14_08670;cds-C4N14_08575;cds-C4N14_08570;cds-C4N14_08525;cds-C4N14_08520;cds-C4N14_08515;cds-C4N14_08450;cds-C4N14_08445;cds-C4N14_08440;cds-C4N14_08435;cds-C4N14_08430;cds-C4N14_08410;cds-C4N14_08400;cds-C4N14_08330;cds-C4N14_08295;cds-C4N14_08265;cds-C4N14_08260;cds-C4N14_08240;cds-C4N14_08230;cds-C4N14_08225;cds-C4N14_08185;cds-C4N14_08155;cds-C4N14_08105;cds-C4N14_07930;cds-C4N14_07925;cds-C4N14_07920;cds-C4N14_07910;cds-C4N14_07905;cds-C4N14_07900;cds-C4N14_07895;cds-C4N14_07890;cds-C4N14_07885;cds-C4N14_07840;cds-C4N14_07815;cds-C4N14_07800;cds-C4N14_07790;cds-C4N14_07725;cds-C4N14_07660;cds-C4N14_07655;cds-C4N14_07620;cds-C4N14_07615;cds-C4N14_07610;cds-C4N14_07605;cds-C4N14_07595;cds-C4N14_07565;cds-C4N14_07560;cds-C4N14_07545;cds-C4N14_07525;cds-C4N14_07510;cds-C4N14_07505;cds-C4N14_07470;cds-C4N14_07415;cds-C4N14_07410;cds-C4N14_07405;cds-C4N14_07380;cds-C4N14_07370;cds-C4N14_07355;cds-C4N14_07345;cds-C4N14_07340;cds-C4N14_07325;cds-C4N14_07315;cds-C4N14_07310;cds-C4N14_07300;cds-C4N14_07290;cds-C4N14_07270;cds-C4N14_07265;cds-C4N14_07250;cds-C4N14_07245;cds-C4N14_07240;cds-C4N14_07235;cds-C4N14_07230;cds-C4N14_07225;cds-C4N14_07220;cds-C4N14_07175;cds-C4N14_07170;cds-C4N14_07165;cds-C4N14_07115;cds-C4N14_07100;cds-C4N14_07095;cds-C4N14_07090;cds-C4N14_07070;cds-C4N14_07025;cds-C4N14_06915;cds-C4N14_06885;cds-C4N14_06875;cds-C4N14_06625;cds-C4N14_06555;cds-C4N14_06535;cds-C4N14_06495;cds-C4N14_06485;cds-C4N14_06480;cds-C4N14_06430;cds-C4N14_06380;cds-C4N14_06365;cds-C4N14_06345;cds-C4N14_06320;cds-C4N14_06310;cds-C4N14_06300;cds-C4N14_06275;cds-C4N14_06270;cds-C4N14_06265;cds-C4N14_06260;cds-C4N14_06200;cds-C4N14_06120;cds-C4N14_06090;cds-C4N14_06075;cds-C4N14_06030;cds-C4N14_06010;cds-C4N14_06005;cds-C4N14_05980;cds-C4N14_05815;cds-C4N14_05800;cds-C4N14_05790;cds-C4N14_05745;cds-C4N14_05620;cds-C4N14_05615;cds-C4N14_05600;cds-C4N14_05580;cds-C4N14_05575;cds-C4N14_05485;cds-C4N14_05480;cds-C4N14_05475;cds-C4N14_05465;cds-C4N14_10135;cds-C4N14_10145;cds-C4N14_10260;cds-C4N14_10310;cds-C4N14_10420;cds-C4N14_10440;cds-C4N14_10455;cds-C4N14_10465;cds-C4N14_10470;cds-C4N14_10475;cds-C4N14_10485;cds-C4N14_10490;cds-C4N14_10495;cds-C4N14_10515;cds-C4N14_10525;cds-C4N14_10535;cds-C4N14_10630;cds-C4N14_10635;cds-C4N14_10640;cds-C4N14_10690;cds-C4N14_10695;cds-C4N14_10700;cds-C4N14_10705;cds-C4N14_10710;cds-C4N14_10715;cds-C4N14_10725;cds-C4N14_10735;cds-C4N14_10740;cds-C4N14_10800;cds-C4N14_10805;cds-C4N14_10835;cds-C4N14_10840;cds-C4N14_10860;cds-C4N14_10865;cds-C4N14_10870;cds-C4N14_10880;cds-C4N14_00055;cds-C4N14_00060;cds-C4N14_00065;cds-C4N14_00070;cds-C4N14_00125;cds-C4N14_00210;cds-C4N14_00215;cds-C4N14_00245;cds-C4N14_00250;cds-C4N14_00370;cds-C4N14_00375;cds-C4N14_00465;cds-C4N14_00585;cds-C4N14_00590;cds-C4N14_00595;cds-C4N14_00605;cds-C4N14_00670;cds-C4N14_00890;cds-C4N14_00950;cds-C4N14_01020;cds-C4N14_01040;cds-C4N14_01055;cds-C4N14_01065;cds-C4N14_01240;cds-C4N14_01245;cds-C4N14_01250;cds-C4N14_01260;cds-C4N14_01265;cds-C4N14_01270;cds-C4N14_01275;cds-C4N14_01280;cds-C4N14_01285;cds-C4N14_01300;cds-C4N14_01305;cds-C4N14_01330;cds-C4N14_01335;cds-C4N14_01340;cds-C4N14_01345;cds-C4N14_01355;cds-C4N14_01360;cds-C4N14_01365;cds-C4N14_01390;cds-C4N14_01395;cds-C4N14_01475;cds-C4N14_01500;cds-C4N14_01505;cds-C4N14_01515;cds-C4N14_01585;cds-C4N14_03870;cds-C4N14_03865;cds-C4N14_03860;cds-C4N14_03840;cds-C4N14_03815;cds-C4N14_03800;cds-C4N14_03790;cds-C4N14_03785;cds-C4N14_03780;cds-C4N14_03755;cds-C4N14_03750;cds-C4N14_03735;cds-C4N14_03730;cds-C4N14_03725;cds-C4N14_03720;cds-C4N14_03680;cds-C4N14_03565;cds-C4N14_03545;cds-C4N14_03530;cds-C4N14_03490;cds-C4N14_03470;cds-C4N14_03425;cds-C4N14_03415;cds-C4N14_03345;cds-C4N14_03065;cds-C4N14_03060;cds-C4N14_02995;cds-C4N14_01845;cds-C4N14_01950;cds-C4N14_02030;cds-C4N14_02045;cds-C4N14_02080;cds-C4N14_02205;cds-C4N14_02210;cds-C4N14_02215</t>
+    <t>cds-C4N14_02390;cds-C4N14_02395;cds-C4N14_02400;cds-C4N14_02450;cds-C4N14_02565;cds-C4N14_02625;cds-C4N14_02635;cds-C4N14_02695;cds-C4N14_02740;cds-C4N14_02745;cds-C4N14_02770;cds-C4N14_02775;cds-C4N14_02780;cds-C4N14_02800;cds-C4N14_02805;cds-C4N14_01785;cds-C4N14_01780;cds-C4N14_04115;cds-C4N14_04120;cds-C4N14_04125;cds-C4N14_04130;cds-C4N14_04135;cds-C4N14_04160;cds-C4N14_04180;cds-C4N14_04250;cds-C4N14_04385;cds-C4N14_04390;cds-C4N14_04395;cds-C4N14_04400;cds-C4N14_04460;cds-C4N14_04570;cds-C4N14_04575;cds-C4N14_04670;cds-C4N14_04695;cds-C4N14_04720;cds-C4N14_04725;cds-C4N14_04745;cds-C4N14_04795;cds-C4N14_04810;cds-C4N14_04815;cds-C4N14_04880;cds-C4N14_04920;cds-C4N14_04955;cds-C4N14_05010;cds-C4N14_05135;cds-C4N14_05140;cds-C4N14_05175;cds-C4N14_05180;cds-C4N14_05185;cds-C4N14_05190;cds-C4N14_05195;cds-C4N14_05200;cds-C4N14_05205;cds-C4N14_05210;cds-C4N14_05215;cds-C4N14_05220;cds-C4N14_05230;cds-C4N14_05240;cds-C4N14_05280;cds-C4N14_10125;cds-C4N14_10115;cds-C4N14_10110;cds-C4N14_10105;cds-C4N14_10085;cds-C4N14_10080;cds-C4N14_10075;cds-C4N14_10070;cds-C4N14_10065;cds-C4N14_10060;cds-C4N14_10055;cds-C4N14_10045;cds-C4N14_10040;cds-C4N14_10035;cds-C4N14_10005;cds-C4N14_09985;cds-C4N14_09965;cds-C4N14_09955;cds-C4N14_09925;cds-C4N14_09835;cds-C4N14_09810;cds-C4N14_09785;cds-C4N14_09770;cds-C4N14_09755;cds-C4N14_09750;cds-C4N14_09725;cds-C4N14_09720;cds-C4N14_09685;cds-C4N14_09605;cds-C4N14_09555;cds-C4N14_09545;cds-C4N14_09540;cds-C4N14_09520;cds-C4N14_09465;cds-C4N14_09430;cds-C4N14_09330;cds-C4N14_09265;cds-C4N14_09260;cds-C4N14_09255;cds-C4N14_09250;cds-C4N14_09245;cds-C4N14_09135;cds-C4N14_09115;cds-C4N14_09020;cds-C4N14_09015;cds-C4N14_09010;cds-C4N14_08980;cds-C4N14_08970;cds-C4N14_08930;cds-C4N14_08920;cds-C4N14_08830;cds-C4N14_08825;cds-C4N14_08805;cds-C4N14_08690;cds-C4N14_08670;cds-C4N14_08575;cds-C4N14_08570;cds-C4N14_08525;cds-C4N14_08520;cds-C4N14_08515;cds-C4N14_08450;cds-C4N14_08445;cds-C4N14_08440;cds-C4N14_08435;cds-C4N14_08430;cds-C4N14_08410;cds-C4N14_08400;cds-C4N14_08330;cds-C4N14_08295;cds-C4N14_08265;cds-C4N14_08260;cds-C4N14_08240;cds-C4N14_08230;cds-C4N14_08225;cds-C4N14_08185;cds-C4N14_08155;cds-C4N14_08105;cds-C4N14_07930;cds-C4N14_07925;cds-C4N14_07920;cds-C4N14_07910;cds-C4N14_07905;cds-C4N14_07900;cds-C4N14_07895;cds-C4N14_07890;cds-C4N14_07885;cds-C4N14_07840;cds-C4N14_07815;cds-C4N14_07800;cds-C4N14_07790;cds-C4N14_07725;cds-C4N14_07660;cds-C4N14_07655;cds-C4N14_07620;cds-C4N14_07615;cds-C4N14_07610;cds-C4N14_07605;cds-C4N14_07595;cds-C4N14_07565;cds-C4N14_07560;cds-C4N14_07545;cds-C4N14_07525;cds-C4N14_07510;cds-C4N14_07505;cds-C4N14_07470;cds-C4N14_07415;cds-C4N14_07410;cds-C4N14_07405;cds-C4N14_07380;cds-C4N14_07370;cds-C4N14_07355;cds-C4N14_07345;cds-C4N14_07340;cds-C4N14_07325;cds-C4N14_07315;cds-C4N14_07310;cds-C4N14_07300;cds-C4N14_07290;cds-C4N14_07270;cds-C4N14_07265;cds-C4N14_07250;cds-C4N14_07245;cds-C4N14_07240;cds-C4N14_07235;cds-C4N14_07230;cds-C4N14_07225;cds-C4N14_07220;cds-C4N14_07175;cds-C4N14_07170;cds-C4N14_07165;cds-C4N14_07115;cds-C4N14_07100;cds-C4N14_07095;cds-C4N14_07090;cds-C4N14_07070;cds-C4N14_07025;cds-C4N14_06915;cds-C4N14_06885;cds-C4N14_06875;cds-C4N14_06625;cds-C4N14_06555;cds-C4N14_06535;cds-C4N14_06495;cds-C4N14_06485;cds-C4N14_06480;cds-C4N14_06430;cds-C4N14_06380;cds-C4N14_06365;cds-C4N14_06345;cds-C4N14_06320;cds-C4N14_06310;cds-C4N14_06300;cds-C4N14_06275;cds-C4N14_06270;cds-C4N14_06265;cds-C4N14_06260;cds-C4N14_06200;cds-C4N14_06120;cds-C4N14_06090;cds-C4N14_06075;cds-C4N14_06030;cds-C4N14_06010;cds-C4N14_06005;cds-C4N14_05980;cds-C4N14_05815;cds-C4N14_05800;cds-C4N14_05790;cds-C4N14_05745;cds-C4N14_05620;cds-C4N14_05615;cds-C4N14_05600;cds-C4N14_05580;cds-C4N14_05575;cds-C4N14_05485;cds-C4N14_05480;cds-C4N14_05475;cds-C4N14_05465;cds-C4N14_10135;cds-C4N14_10145;cds-C4N14_10260;cds-C4N14_10310;cds-C4N14_10420;cds-C4N14_10440;cds-C4N14_10455;cds-C4N14_10465;cds-C4N14_10470;cds-C4N14_10475;cds-C4N14_10485;cds-C4N14_10490;cds-C4N14_10495;cds-C4N14_10515;cds-C4N14_10525;cds-C4N14_10535;cds-C4N14_10630;cds-C4N14_10635;cds-C4N14_10640;cds-C4N14_10690;cds-C4N14_10695;cds-C4N14_10700;cds-C4N14_10705;cds-C4N14_10710;cds-C4N14_10715;cds-C4N14_10725;cds-C4N14_10735;cds-C4N14_10740;cds-C4N14_10800;cds-C4N14_10805;cds-C4N14_10835;cds-C4N14_10840;cds-C4N14_10860;cds-C4N14_10865;cds-C4N14_10870;cds-C4N14_10880;cds-C4N14_00055;cds-C4N14_00060;cds-C4N14_00065;cds-C4N14_00070;cds-C4N14_00125;cds-C4N14_00210;cds-C4N14_00215;cds-C4N14_00245;cds-C4N14_00250;cds-C4N14_00370;cds-C4N14_00375;cds-C4N14_00465;cds-C4N14_00585;cds-C4N14_00590;cds-C4N14_00595;cds-C4N14_00605;cds-C4N14_00670;cds-C4N14_00890;cds-C4N14_00950;cds-C4N14_01020;cds-C4N14_01040;cds-C4N14_01055;cds-C4N14_01065;cds-C4N14_01240;cds-C4N14_01245;cds-C4N14_01250;cds-C4N14_01260;cds-C4N14_01265;cds-C4N14_01270;cds-C4N14_01275;cds-C4N14_01280;cds-C4N14_01285;cds-C4N14_01300;cds-C4N14_01305;cds-C4N14_01330;cds-C4N14_01335;cds-C4N14_01340;cds-C4N14_01345;cds-C4N14_01355;cds-C4N14_01360;cds-C4N14_01365;cds-C4N14_01390;cds-C4N14_01395;cds-C4N14_01475;cds-C4N14_01500;cds-C4N14_01505;cds-C4N14_01515;cds-C4N14_01585;cds-C4N14_03870;cds-C4N14_03865;cds-C4N14_03860;cds-C4N14_03840;cds-C4N14_03815;cds-C4N14_03800;cds-C4N14_03790;cds-C4N14_03785;cds-C4N14_03780;cds-C4N14_03755;cds-C4N14_03750;cds-C4N14_03735;cds-C4N14_03730;cds-C4N14_03725;cds-C4N14_03720;cds-C4N14_03680;cds-C4N14_03565;cds-C4N14_03545;cds-C4N14_03530;cds-C4N14_03490;cds-C4N14_03470;cds-C4N14_03425;cds-C4N14_03415;cds-C4N14_03345;cds-C4N14_03065;cds-C4N14_03060;cds-C4N14_02995;cds-C4N14_01845;cds-C4N14_01950;cds-C4N14_02030;cds-C4N14_02045;cds-C4N14_02080;cds-C4N14_02205;cds-C4N14_02210;cds-C4N14_02215</t>
   </si>
   <si>
     <t>cds-C4N14_02800;cds-C4N14_04385;cds-C4N14_04670;cds-C4N14_05180;cds-C4N14_10115;cds-C4N14_10110;cds-C4N14_09955;cds-C4N14_09750;cds-C4N14_09685;cds-C4N14_08240;cds-C4N14_06915;cds-C4N14_06555;cds-C4N14_06310;cds-C4N14_06275;cds-C4N14_06270;cds-C4N14_06265;cds-C4N14_06260;cds-C4N14_10310;cds-C4N14_10535;cds-C4N14_00215;cds-C4N14_01395</t>
@@ -773,7 +773,7 @@
     <t>cds-C4N14_04120;cds-C4N14_04125;cds-C4N14_04135;cds-C4N14_04250;cds-C4N14_10115;cds-C4N14_10110;cds-C4N14_09755;cds-C4N14_09260;cds-C4N14_07840;cds-C4N14_06535;cds-C4N14_03815</t>
   </si>
   <si>
-    <t>cds-C4N14_04330;cds-C4N14_04490;cds-C4N14_04495;cds-C4N14_04720;cds-C4N14_04725;cds-C4N14_04990;cds-C4N14_04995;cds-C4N14_09750;cds-C4N14_05830;cds-C4N14_05825;cds-C4N14_10315;cds-C4N14_10320;cds-C4N14_10325;cds-C4N14_10330;cds-C4N14_10420;cds-C4N14_03785;cds-C4N14_03780;cds-C4N14_03775;cds-C4N14_02185;cds-C4N14_02190;cds-C4N14_02195</t>
+    <t>cds-C4N14_04330;cds-C4N14_04490;cds-C4N14_04495;cds-C4N14_04720;cds-C4N14_04725;cds-C4N14_04990;cds-C4N14_04995;cds-C4N14_09750;cds-C4N14_05830;cds-C4N14_05825;cds-C4N14_05765;cds-C4N14_10315;cds-C4N14_10320;cds-C4N14_10325;cds-C4N14_10330;cds-C4N14_10420;cds-C4N14_03785;cds-C4N14_03780;cds-C4N14_03775;cds-C4N14_02185;cds-C4N14_02190;cds-C4N14_02195</t>
   </si>
   <si>
     <t>cds-C4N14_05280;cds-C4N14_05800;cds-C4N14_05615;cds-C4N14_00890;cds-C4N14_00950;cds-C4N14_01020;cds-C4N14_03065;cds-C4N14_02215</t>
@@ -785,7 +785,7 @@
     <t>cds-C4N14_04720;cds-C4N14_04725;cds-C4N14_09955;cds-C4N14_09750;cds-C4N14_03785;cds-C4N14_03780;cds-C4N14_03755;cds-C4N14_03750;cds-C4N14_03735;cds-C4N14_03730;cds-C4N14_03725;cds-C4N14_03720</t>
   </si>
   <si>
-    <t>cds-C4N14_04115;cds-C4N14_09955;cds-C4N14_09805;cds-C4N14_09555;cds-C4N14_03870;cds-C4N14_03865;cds-C4N14_03860</t>
+    <t>cds-C4N14_04115;cds-C4N14_09955;cds-C4N14_09555;cds-C4N14_03870;cds-C4N14_03865;cds-C4N14_03860</t>
   </si>
   <si>
     <t>cds-C4N14_05615;cds-C4N14_00890;cds-C4N14_01020</t>
@@ -869,15 +869,15 @@
     <t>cds-C4N14_09955;cds-C4N14_09725;cds-C4N14_08445;cds-C4N14_06875;cds-C4N14_06380</t>
   </si>
   <si>
+    <t>cds-C4N14_09855;cds-C4N14_09605;cds-C4N14_06365;cds-C4N14_06075;cds-C4N14_05765;cds-C4N14_05760;cds-C4N14_05755;cds-C4N14_00485</t>
+  </si>
+  <si>
     <t>cds-C4N14_04180;cds-C4N14_05175;cds-C4N14_09115;cds-C4N14_07095;cds-C4N14_06885;cds-C4N14_06625;cds-C4N14_06380;cds-C4N14_06275;cds-C4N14_06030;cds-C4N14_10490;cds-C4N14_10495;cds-C4N14_10525;cds-C4N14_00370;cds-C4N14_01300;cds-C4N14_01305</t>
   </si>
   <si>
     <t>cds-C4N14_09430;cds-C4N14_06300;cds-C4N14_05615;cds-C4N14_00890;cds-C4N14_01020</t>
   </si>
   <si>
-    <t>cds-C4N14_09855;cds-C4N14_09605;cds-C4N14_06365;cds-C4N14_06075;cds-C4N14_05760;cds-C4N14_05755;cds-C4N14_00485</t>
-  </si>
-  <si>
     <t>cds-C4N14_05280;cds-C4N14_10105;cds-C4N14_09430;cds-C4N14_06300;cds-C4N14_05800;cds-C4N14_01055;cds-C4N14_02205;cds-C4N14_02210;cds-C4N14_02215</t>
   </si>
   <si>
@@ -890,7 +890,7 @@
     <t>cds-C4N14_04125;cds-C4N14_10145</t>
   </si>
   <si>
-    <t>cds-C4N14_09855;cds-C4N14_09255;cds-C4N14_05760;cds-C4N14_05755;cds-C4N14_05430</t>
+    <t>cds-C4N14_09855;cds-C4N14_09255;cds-C4N14_05765;cds-C4N14_05760;cds-C4N14_05755;cds-C4N14_05430</t>
   </si>
   <si>
     <t>cds-C4N14_05905;cds-C4N14_01035</t>
@@ -985,7 +985,7 @@
         <v>3.118702510104315E-8</v>
       </c>
       <c r="E2" t="n">
-        <v>2.4492561749638744E-6</v>
+        <v>2.3379419095053504E-6</v>
       </c>
       <c r="F2" t="n">
         <v>1.0492062423686906E-8</v>
@@ -1014,7 +1014,7 @@
         <v>6.024662789391541E-8</v>
       </c>
       <c r="E3" t="n">
-        <v>2.4492561749638744E-6</v>
+        <v>2.3379419095053504E-6</v>
       </c>
       <c r="F3" t="n">
         <v>2.222203470992412E-8</v>
@@ -1043,7 +1043,7 @@
         <v>7.734493184096446E-8</v>
       </c>
       <c r="E4" t="n">
-        <v>2.4492561749638744E-6</v>
+        <v>2.3379419095053504E-6</v>
       </c>
       <c r="F4" t="n">
         <v>0.20968105746716587</v>
@@ -1063,22 +1063,22 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>20.0</v>
+        <v>14.0</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D5" t="n">
-        <v>2.537235246748634E-7</v>
+        <v>9.84396593475937E-8</v>
       </c>
       <c r="E5" t="n">
-        <v>6.025933711028006E-6</v>
+        <v>2.3379419095053504E-6</v>
       </c>
       <c r="F5" t="n">
-        <v>6.313183199375452E-13</v>
+        <v>5.088907095896801E-12</v>
       </c>
       <c r="G5" t="n">
-        <v>9.995873399011133E-12</v>
+        <v>4.028718117584967E-11</v>
       </c>
       <c r="H5" t="s">
         <v>108</v>
@@ -1092,22 +1092,22 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>13.0</v>
+        <v>20.0</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" t="n">
-        <v>5.699480170183265E-7</v>
+        <v>2.537235246748634E-7</v>
       </c>
       <c r="E6" t="n">
-        <v>1.0829012323348202E-5</v>
+        <v>4.820746968822404E-6</v>
       </c>
       <c r="F6" t="n">
-        <v>1.2129185799125542E-11</v>
+        <v>6.313183199375452E-13</v>
       </c>
       <c r="G6" t="n">
-        <v>9.602272090974388E-11</v>
+        <v>9.995873399011133E-12</v>
       </c>
       <c r="H6" t="s">
         <v>109</v>
@@ -1136,7 +1136,7 @@
         <v>2.2836197717035845E-12</v>
       </c>
       <c r="G7" t="n">
-        <v>2.4355974513270633E-11</v>
+        <v>2.480173516231357E-11</v>
       </c>
       <c r="H7" t="s">
         <v>110</v>
@@ -1368,7 +1368,7 @@
         <v>2.068487754954616E-5</v>
       </c>
       <c r="G15" t="n">
-        <v>3.509041727155152E-5</v>
+        <v>3.447479591591027E-5</v>
       </c>
       <c r="H15" t="s">
         <v>117</v>
@@ -1449,13 +1449,13 @@
         <v>9.220751580354018E-6</v>
       </c>
       <c r="E18" t="n">
-        <v>5.0792929788510484E-5</v>
+        <v>5.107640719249817E-5</v>
       </c>
       <c r="F18" t="n">
         <v>1.7958311539144142E-5</v>
       </c>
       <c r="G18" t="n">
-        <v>3.101890174943079E-5</v>
+        <v>3.0464992789619528E-5</v>
       </c>
       <c r="H18" t="s">
         <v>120</v>
@@ -1478,13 +1478,13 @@
         <v>9.677635046999654E-6</v>
       </c>
       <c r="E19" t="n">
-        <v>5.0792929788510484E-5</v>
+        <v>5.107640719249817E-5</v>
       </c>
       <c r="F19" t="n">
         <v>0.09022046602117231</v>
       </c>
       <c r="G19" t="n">
-        <v>0.10988390092322269</v>
+        <v>0.10849296546849835</v>
       </c>
       <c r="H19" t="s">
         <v>121</v>
@@ -1498,22 +1498,22 @@
         <v>26</v>
       </c>
       <c r="B20" t="n">
-        <v>356.0</v>
+        <v>355.0</v>
       </c>
       <c r="C20" t="s">
         <v>103</v>
       </c>
       <c r="D20" t="n">
-        <v>1.0158585957702097E-5</v>
+        <v>1.0259965088563022E-5</v>
       </c>
       <c r="E20" t="n">
-        <v>5.0792929788510484E-5</v>
+        <v>5.119604252784571E-5</v>
       </c>
       <c r="F20" t="n">
-        <v>2.307408111783534E-12</v>
+        <v>2.3496380680086543E-12</v>
       </c>
       <c r="G20" t="n">
-        <v>2.4355974513270633E-11</v>
+        <v>2.480173516231357E-11</v>
       </c>
       <c r="H20" t="s">
         <v>122</v>
@@ -1745,7 +1745,7 @@
         <v>4.825183036048958E-9</v>
       </c>
       <c r="G28" t="n">
-        <v>1.6371156729451822E-8</v>
+        <v>1.6977495867579666E-8</v>
       </c>
       <c r="H28" t="s">
         <v>130</v>
@@ -1919,7 +1919,7 @@
         <v>7.86587697751729E-6</v>
       </c>
       <c r="G34" t="n">
-        <v>1.383811690489153E-5</v>
+        <v>1.3586514779348046E-5</v>
       </c>
       <c r="H34" t="s">
         <v>136</v>
@@ -2209,7 +2209,7 @@
         <v>0.006119214310630527</v>
       </c>
       <c r="G44" t="n">
-        <v>0.008807959992574244</v>
+        <v>0.008943467069383077</v>
       </c>
       <c r="H44" t="s">
         <v>146</v>
@@ -2383,7 +2383,7 @@
         <v>0.00874419917908365</v>
       </c>
       <c r="G50" t="n">
-        <v>0.012398491373327564</v>
+        <v>0.012586347303226466</v>
       </c>
       <c r="H50" t="s">
         <v>152</v>
@@ -2542,22 +2542,22 @@
         <v>62</v>
       </c>
       <c r="B56" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="C56" t="s">
         <v>103</v>
       </c>
       <c r="D56" t="n">
-        <v>9.046732143172543E-4</v>
+        <v>0.00134999240876084</v>
       </c>
       <c r="E56" t="n">
-        <v>0.0015626173701843483</v>
+        <v>0.0023318050696778145</v>
       </c>
       <c r="F56" t="n">
-        <v>4.316640926772654E-9</v>
+        <v>5.531496605322563E-9</v>
       </c>
       <c r="G56" t="n">
-        <v>1.5188181038644523E-8</v>
+        <v>1.8767577768058693E-8</v>
       </c>
       <c r="H56" t="s">
         <v>158</v>
@@ -2658,22 +2658,22 @@
         <v>66</v>
       </c>
       <c r="B60" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C60" t="s">
         <v>103</v>
       </c>
       <c r="D60" t="n">
-        <v>0.004841837502421171</v>
+        <v>0.006038987932431896</v>
       </c>
       <c r="E60" t="n">
-        <v>0.007796179029322225</v>
+        <v>0.009723794128492036</v>
       </c>
       <c r="F60" t="n">
-        <v>0.004504672786113611</v>
+        <v>0.014433251327414846</v>
       </c>
       <c r="G60" t="n">
-        <v>0.006583752533550662</v>
+        <v>0.020164101119182504</v>
       </c>
       <c r="H60" t="s">
         <v>162</v>
@@ -3021,7 +3021,7 @@
         <v>5.051461705951851E-6</v>
       </c>
       <c r="G72" t="n">
-        <v>9.054506831423129E-6</v>
+        <v>8.886830778989367E-6</v>
       </c>
       <c r="H72" t="s">
         <v>174</v>
@@ -3470,22 +3470,22 @@
         <v>94</v>
       </c>
       <c r="B88" t="n">
-        <v>15.0</v>
+        <v>8.0</v>
       </c>
       <c r="C88" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D88" t="n">
-        <v>0.3447663048050713</v>
+        <v>0.3066127122433679</v>
       </c>
       <c r="E88" t="n">
-        <v>0.37646895352277904</v>
+        <v>0.3348069846335627</v>
       </c>
       <c r="F88" t="n">
-        <v>2.1328433056550592E-10</v>
+        <v>3.077359651526373E-6</v>
       </c>
       <c r="G88" t="n">
-        <v>9.648576858915744E-10</v>
+        <v>5.516022016886896E-6</v>
       </c>
       <c r="H88" t="s">
         <v>190</v>
@@ -3499,22 +3499,22 @@
         <v>95</v>
       </c>
       <c r="B89" t="n">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="C89" t="s">
         <v>103</v>
       </c>
       <c r="D89" t="n">
-        <v>0.3539796858489064</v>
+        <v>0.3447663048050713</v>
       </c>
       <c r="E89" t="n">
-        <v>0.3785962064175837</v>
+        <v>0.37219089723274745</v>
       </c>
       <c r="F89" t="n">
-        <v>0.011534179240549754</v>
+        <v>2.1328433056550592E-10</v>
       </c>
       <c r="G89" t="n">
-        <v>0.0161139268801798</v>
+        <v>9.648576858915744E-10</v>
       </c>
       <c r="H89" t="s">
         <v>191</v>
@@ -3528,22 +3528,22 @@
         <v>96</v>
       </c>
       <c r="B90" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="C90" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D90" t="n">
-        <v>0.3546848670648942</v>
+        <v>0.3539796858489064</v>
       </c>
       <c r="E90" t="n">
-        <v>0.3785962064175837</v>
+        <v>0.37784348489490005</v>
       </c>
       <c r="F90" t="n">
-        <v>2.2835023362892656E-5</v>
+        <v>0.011534179240549754</v>
       </c>
       <c r="G90" t="n">
-        <v>3.805837227148776E-5</v>
+        <v>0.01635443325152577</v>
       </c>
       <c r="H90" t="s">
         <v>192</v>
@@ -3673,22 +3673,22 @@
         <v>101</v>
       </c>
       <c r="B95" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C95" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D95" t="n">
-        <v>0.9033170508293076</v>
+        <v>0.7707494995739655</v>
       </c>
       <c r="E95" t="n">
-        <v>0.9125733491283992</v>
+        <v>0.7789489623353908</v>
       </c>
       <c r="F95" t="n">
-        <v>0.09158356829225249</v>
+        <v>0.07097349274490315</v>
       </c>
       <c r="G95" t="n">
-        <v>0.11013213908562008</v>
+        <v>0.08644207449699742</v>
       </c>
       <c r="H95" t="s">
         <v>197</v>

</xml_diff>